<commit_message>
chart with calling functions
</commit_message>
<xml_diff>
--- a/transactions.xlsx
+++ b/transactions.xlsx
@@ -139,6 +139,11 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
+          <cat>
+            <numRef>
+              <f>'Sheet1'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
           <val>
             <numRef>
               <f>'Sheet1'!$D$2:$D$4</f>
@@ -530,7 +535,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.2"/>

</xml_diff>